<commit_message>
avance sobre gestion de cachedificaciones
agregado de densidades
</commit_message>
<xml_diff>
--- a/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_glass_D25_R25_Pentropia.xlsx
+++ b/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_glass_D25_R25_Pentropia.xlsx
@@ -584,7 +584,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G2" t="n">
         <v>0.2857142857142857</v>
@@ -625,7 +625,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>[0.36870282705068963, 0.571254182457916, 0.8399570029762644, 0.7188030116408483, 0.915922586578981, 0.9643759308650648, 0.8161088220553884]</t>
+          <t>[0.3686896860599518, 0.5712586641311646, 0.8399618864059448, 0.7188007235527039, 0.9159262180328369, 0.964373767375946, 0.8161059021949768]</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -635,14 +635,14 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>[0.36870282705068963, 0.9643759308650648, 1.1263236539931059, 1.2241735099679416, 1.2196421966004263, 1.470400260947273, 1.5570746533140791]</t>
+          <t>[0.3686896860599518, 0.964373767375946, 1.126319169998169, 1.2241731882095337, 1.2196450233459473, 1.4703971147537231, 1.557084560394287]</t>
         </is>
       </c>
       <c r="U2" t="n">
         <v>2</v>
       </c>
       <c r="V2" t="n">
-        <v>0.5705852098823702</v>
+        <v>0.5705868005752563</v>
       </c>
       <c r="W2" t="n">
         <v>0</v>
@@ -651,7 +651,7 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.112968</t>
+          <t>2025-10-17T02:10:07.542671</t>
         </is>
       </c>
     </row>
@@ -674,7 +674,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G3" t="n">
         <v>0.2857142857142857</v>
@@ -715,7 +715,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>[0.29108793636307856, 0.3007785898777099, 0.5837685871344127, 0.6349888467834518, 0.6392179051246156, 0.5765435063524058, 0.6429941276074913]</t>
+          <t>[0.29108816385269165, 0.3007749617099762, 0.5837634801864624, 0.6349945664405823, 0.639224112033844, 0.5765426754951477, 0.6429972052574158]</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -725,14 +725,14 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>[0.6392179051246156, 0.7289855999382798, 0.8478721364650169, 0.9712824467055972, 1.0848981146158845, 1.3480260842400091, 1.2196421966004263]</t>
+          <t>[0.639224112033844, 0.7289791107177734, 0.8478673100471497, 0.9712804555892944, 1.0848945379257202, 1.3480218648910522, 1.2196450233459473]</t>
         </is>
       </c>
       <c r="U3" t="n">
         <v>2</v>
       </c>
       <c r="V3" t="n">
-        <v>0.537080536684876</v>
+        <v>0.537077784538269</v>
       </c>
       <c r="W3" t="n">
         <v>4</v>
@@ -745,7 +745,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.112968</t>
+          <t>2025-10-17T02:10:07.543667</t>
         </is>
       </c>
     </row>
@@ -768,7 +768,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G4" t="n">
         <v>0.2857142857142857</v>
@@ -809,7 +809,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>[1.5354786819005746, 1.5763796645421633, 1.518245731033573, 1.601565229324348, 1.8141893925589672, 2.4762693355922436, 1.6455757268203273]</t>
+          <t>[1.5354762077331543, 1.5763767957687378, 1.5182515382766724, 1.6015644073486328, 1.814195990562439, 2.4762635231018066, 1.645581841468811]</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -819,14 +819,14 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>[2.4762693355922436, 2.9099357041697727, 2.5544267277225856, 3.135508093288406, 2.661673534050169, 2.6628466326195666, 2.9838959810785206]</t>
+          <t>[2.4762635231018066, 2.9099297523498535, 2.5544352531433105, 3.1355085372924805, 2.66167950630188, 2.662851095199585, 2.9838945865631104]</t>
         </is>
       </c>
       <c r="U4" t="n">
         <v>2</v>
       </c>
       <c r="V4" t="n">
-        <v>0.7247190868889184</v>
+        <v>0.724717378616333</v>
       </c>
       <c r="W4" t="n">
         <v>4</v>
@@ -839,7 +839,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.112968</t>
+          <t>2025-10-17T02:10:07.543667</t>
         </is>
       </c>
     </row>
@@ -862,7 +862,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G5" t="n">
         <v>0.2857142857142857</v>
@@ -903,7 +903,7 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>[0.46185233475496995, 0.46297917576952363, 0.7553792977804442, 0.8820956202336345, 0.8820956202336345, 1.2559472641199887, 1.800462053004792]</t>
+          <t>[0.4618493616580963, 0.46296268701553345, 0.7553806304931641, 0.8820913434028625, 0.8820913434028625, 1.2559460401535034, 1.8004459142684937]</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -913,14 +913,14 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>[0.7553792977804442, 2.353507723745344, 3.135508093288406, 3.852336164887893, 2.6655485707291344, 2.417296510745149, 2.481662343266953]</t>
+          <t>[0.7553806304931641, 2.353519916534424, 3.1355085372924805, 3.852335214614868, 2.665560245513916, 2.4172964096069336, 2.481671094894409]</t>
         </is>
       </c>
       <c r="U5" t="n">
         <v>2</v>
       </c>
       <c r="V5" t="n">
-        <v>0.3056115418193889</v>
+        <v>0.3056077361106873</v>
       </c>
       <c r="W5" t="n">
         <v>2</v>
@@ -933,7 +933,7 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.112968</t>
+          <t>2025-10-17T02:10:07.543667</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G6" t="n">
         <v>0.2857142857142857</v>
@@ -997,7 +997,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>[0.9198494393336901, 0.9164440119967676, 1.015355534006097, 0.9643759308650648, 1.1352381971484793, 1.309078032215393, 1.2096121380822629]</t>
+          <t>[0.9198511242866516, 0.9164473414421082, 1.0153549909591675, 0.964373767375946, 1.1352434158325195, 1.3090776205062866, 1.209598422050476]</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1007,14 +1007,14 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>[0.9643759308650648, 1.015355534006097, 1.309078032215393, 1.6240327394665033, 1.7274423917541522, 1.9255385383437427, 1.6671735468792106]</t>
+          <t>[0.964373767375946, 1.0153549909591675, 1.3090776205062866, 1.624017596244812, 1.7274311780929565, 1.9255344867706299, 1.6671695709228516]</t>
         </is>
       </c>
       <c r="U6" t="n">
         <v>2</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7060023456084124</v>
+        <v>0.7060033082962036</v>
       </c>
       <c r="W6" t="n">
         <v>0</v>
@@ -1023,7 +1023,7 @@
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.112968</t>
+          <t>2025-10-17T02:10:07.543667</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G7" t="n">
         <v>0.2857142857142857</v>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>[1.0445740521454645, 0.7342474404872175, 1.350972587814987, 0.9219694314401171, 0.9574600932486723, 1.0273458703387217, 0.8839927453713303]</t>
+          <t>[1.0445706844329834, 0.7342439293861389, 1.3509747982025146, 0.9219695329666138, 0.9574594497680664, 1.027353048324585, 0.8839975595474243]</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1097,14 +1097,14 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>[1.015057799175586, 1.0873292441229583, 1.1586569849203083, 1.3480260842400091, 1.470400260947273, 1.4868313662359702, 2.2044641100359974]</t>
+          <t>[1.0150388479232788, 1.0873119831085205, 1.158658742904663, 1.3480218648910522, 1.4703971147537231, 1.486830234527588, 2.204462766647339]</t>
         </is>
       </c>
       <c r="U7" t="n">
         <v>2</v>
       </c>
       <c r="V7" t="n">
-        <v>0.7479950354889064</v>
+        <v>0.7479963302612305</v>
       </c>
       <c r="W7" t="n">
         <v>2</v>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.112968</t>
+          <t>2025-10-17T02:10:07.543667</t>
         </is>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G8" t="n">
         <v>0.2857142857142857</v>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>[0.290743137515647, 0.285043916571243, 0.30986970738125885, 0.4762486808158445, 0.6092232120953457, 0.6937357956386917, 0.6997585091441121]</t>
+          <t>[0.2907591462135315, 0.28504446148872375, 0.3098526895046234, 0.4762324094772339, 0.6092221736907959, 0.693737268447876, 0.6997390985488892]</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1191,14 +1191,14 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>[0.285043916571243, 0.6743329932424019, 0.8478721364650169, 1.015057799175586, 1.2241735099679416, 1.3019104729087863, 1.6027152759797092]</t>
+          <t>[0.28504446148872375, 0.6743265986442566, 0.8478673100471497, 1.0150388479232788, 1.2241731882095337, 1.3018968105316162, 1.6027143001556396]</t>
         </is>
       </c>
       <c r="U8" t="n">
         <v>2</v>
       </c>
       <c r="V8" t="n">
-        <v>0.3091033016980365</v>
+        <v>0.3090955018997192</v>
       </c>
       <c r="W8" t="n">
         <v>2</v>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.113967</t>
+          <t>2025-10-17T02:10:07.543667</t>
         </is>
       </c>
     </row>
@@ -1234,7 +1234,7 @@
         <v>7</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G9" t="n">
         <v>0.2857142857142857</v>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>[0.36870282705068963, 0.5519547370633832, 0.7350731770769507, 0.7528594013729141, 1.015355534006097, 0.8294772913953069, 1.0044478913104573]</t>
+          <t>[0.3686896860599518, 0.5519679188728333, 0.735078752040863, 0.7528611421585083, 1.0153549909591675, 0.8294775485992432, 1.004456877708435]</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1285,14 +1285,14 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>[0.36870282705068963, 1.015355534006097, 1.0848981146158845, 1.1840853595030576, 1.3019104729087863, 1.4868313662359702, 1.475155267747228]</t>
+          <t>[0.3686896860599518, 1.0153549909591675, 1.0848945379257202, 1.1840670108795166, 1.3018968105316162, 1.486830234527588, 1.4751609563827515]</t>
         </is>
       </c>
       <c r="U9" t="n">
         <v>2</v>
       </c>
       <c r="V9" t="n">
-        <v>0.5843602167132588</v>
+        <v>0.584369421005249</v>
       </c>
       <c r="W9" t="n">
         <v>0</v>
@@ -1301,7 +1301,7 @@
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.113967</t>
+          <t>2025-10-17T02:10:07.543667</t>
         </is>
       </c>
     </row>
@@ -1324,7 +1324,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G10" t="n">
         <v>0.2857142857142857</v>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>[0.285043916571243, 0.3613020375403079, 0.3682554256573937, 0.38688552012503286, 0.5760992767784409, 0.6288485199178419, 0.567023673930235]</t>
+          <t>[0.28504446148872375, 0.36131569743156433, 0.36825448274612427, 0.38687416911125183, 0.5760982632637024, 0.6288474202156067, 0.5670149326324463]</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -1375,14 +1375,14 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>[0.285043916571243, 0.6349515184349481, 0.7289855999382798, 1.0873292441229583, 1.1263236539931059, 1.1840853595030576, 1.475092862204293]</t>
+          <t>[0.28504446148872375, 0.6349484324455261, 0.7289791107177734, 1.0873119831085205, 1.126319169998169, 1.1840670108795166, 1.4750926494598389]</t>
         </is>
       </c>
       <c r="U10" t="n">
         <v>2</v>
       </c>
       <c r="V10" t="n">
-        <v>0.3809025155488346</v>
+        <v>0.3809074759483337</v>
       </c>
       <c r="W10" t="n">
         <v>5</v>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.113967</t>
+          <t>2025-10-17T02:10:07.543667</t>
         </is>
       </c>
     </row>
@@ -1418,7 +1418,7 @@
         <v>7</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G11" t="n">
         <v>0.2857142857142857</v>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>[0.39793813337752815, 0.3796159808557999, 0.547131824675983, 0.5109725664891919, 0.466880727756286, 0.5868905832144952, 0.6392179051246156]</t>
+          <t>[0.39794325828552246, 0.3796297311782837, 0.5471352934837341, 0.5109684467315674, 0.4668952524662018, 0.5869107246398926, 0.639224112033844]</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -1469,14 +1469,14 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>[0.6349515184349481, 0.6743329932424019, 0.6392179051246156, 1.1125232778579464, 1.1586569849203083, 1.475155267747228, 1.5570746533140791]</t>
+          <t>[0.6349484324455261, 0.6743265986442566, 0.639224112033844, 1.1125237941741943, 1.158658742904663, 1.4751609563827515, 1.557084560394287]</t>
         </is>
       </c>
       <c r="U11" t="n">
         <v>2</v>
       </c>
       <c r="V11" t="n">
-        <v>0.5016346664722884</v>
+        <v>0.5016424655914307</v>
       </c>
       <c r="W11" t="n">
         <v>4</v>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.113967</t>
+          <t>2025-10-17T02:10:07.543667</t>
         </is>
       </c>
     </row>
@@ -1512,7 +1512,7 @@
         <v>7</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G12" t="n">
         <v>0.2857142857142857</v>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>[1.022522729127132, 0.7418466361563256, 1.091730518109694, 0.8169284393537438, 0.9712824467055972, 0.8513187214136887, 0.9974814909302543]</t>
+          <t>[1.022521734237671, 0.7418535351753235, 1.0917242765426636, 0.8169267773628235, 0.9712804555892944, 0.8513126373291016, 0.9974803328514099]</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -1563,14 +1563,14 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>[0.9712824467055972, 1.1125232778579464, 1.475092862204293, 1.6027152759797092, 2.0702255154153795, 1.9131038424109268, 2.3420474164918956]</t>
+          <t>[0.9712804555892944, 1.1125237941741943, 1.4750926494598389, 1.6027143001556396, 2.070220708847046, 1.913097858428955, 2.342046022415161]</t>
         </is>
       </c>
       <c r="U12" t="n">
         <v>2</v>
       </c>
       <c r="V12" t="n">
-        <v>0.7366058472070856</v>
+        <v>0.7366058826446533</v>
       </c>
       <c r="W12" t="n">
         <v>3</v>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.114966</t>
+          <t>2025-10-17T02:10:07.543667</t>
         </is>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
         <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G13" t="n">
         <v>0.2857142857142857</v>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>[1.9609936844987668, 2.4762693355922436, 2.5488143551159124, 3.9857840791532855, 2.814430996857044, 2.781341715903314, 3.241391020906572]</t>
+          <t>[1.961000919342041, 2.4762635231018066, 2.548816442489624, 3.9857804775238037, 2.8144288063049316, 2.781341075897217, 3.2413923740386963]</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -1657,14 +1657,14 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>[2.4762693355922436, 3.852336164887893, 3.940240431990059, 3.849267075737102, 3.735630166896788, 4.553111058292238, 4.460374817552124]</t>
+          <t>[2.4762635231018066, 3.852335214614868, 3.940241575241089, 3.849271774291992, 3.7356345653533936, 4.5531134605407715, 4.46036958694458]</t>
         </is>
       </c>
       <c r="U13" t="n">
         <v>2</v>
       </c>
       <c r="V13" t="n">
-        <v>0.9301217412676031</v>
+        <v>0.9301201105117798</v>
       </c>
       <c r="W13" t="n">
         <v>3</v>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.114966</t>
+          <t>2025-10-17T02:10:07.544665</t>
         </is>
       </c>
     </row>
@@ -1700,7 +1700,7 @@
         <v>7</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G14" t="n">
         <v>0.2857142857142857</v>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>[0.44201139323274474, 0.44201139323274474, 0.7553792977804442, 0.817289129845502, 1.0266676237864174, 1.20002024796093, 1.2940247242682115]</t>
+          <t>[0.4420248568058014, 0.4420248568058014, 0.7553806304931641, 0.8172926902770996, 1.0266729593276978, 1.2000261545181274, 1.2940304279327393]</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
@@ -1751,14 +1751,14 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>[0.7553792977804442, 2.2044641100359974, 2.9099357041697727, 3.940240431990059, 2.5074243448209392, 2.7999065735366058, 2.5194056150095907]</t>
+          <t>[0.7553806304931641, 2.204462766647339, 2.9099297523498535, 3.940241575241089, 2.5074117183685303, 2.7999069690704346, 2.5194039344787598]</t>
         </is>
       </c>
       <c r="U14" t="n">
         <v>2</v>
       </c>
       <c r="V14" t="n">
-        <v>0.2917710734144828</v>
+        <v>0.291774183511734</v>
       </c>
       <c r="W14" t="n">
         <v>3</v>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.114966</t>
+          <t>2025-10-17T02:10:07.544665</t>
         </is>
       </c>
     </row>
@@ -1794,7 +1794,7 @@
         <v>7</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6160589902502255</v>
+        <v>0.6160572926326269</v>
       </c>
       <c r="G15" t="n">
         <v>0.2857142857142857</v>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>[0.8769890823808907, 0.9809583086635929, 0.9985459325462515, 1.3458586455349735, 1.1135126667475501, 1.1277871921736737, 1.309078032215393]</t>
+          <t>[0.8769850134849548, 0.9809556007385254, 0.998561441898346, 1.3458682298660278, 1.1135129928588867, 1.1277869939804077, 1.3090776205062866]</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
@@ -1845,14 +1845,14 @@
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>[1.309078032215393, 2.5544267277225856, 2.015712067298128, 2.3420474164918956, 1.9811919545498997, 1.9998280260557344, 2.1122709618390516]</t>
+          <t>[1.3090776205062866, 2.5544352531433105, 2.0157172679901123, 2.342046022415161, 1.981188416481018, 1.9998292922973633, 2.1122682094573975]</t>
         </is>
       </c>
       <c r="U15" t="n">
         <v>2</v>
       </c>
       <c r="V15" t="n">
-        <v>0.6579989401491165</v>
+        <v>0.6580042839050293</v>
       </c>
       <c r="W15" t="n">
         <v>2</v>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.114966</t>
+          <t>2025-10-17T02:10:07.544665</t>
         </is>
       </c>
     </row>
@@ -1888,7 +1888,7 @@
         <v>7</v>
       </c>
       <c r="F16" t="n">
-        <v>0.4762475941271153</v>
+        <v>0.476247085334295</v>
       </c>
       <c r="G16" t="n">
         <v>0.2857142857142857</v>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>[3.548220758848561, 8.691211386839777, 5.758371013344655, 6.487488755518677, 9.90292972678089, 6.694373693143342, 5.858822564490876]</t>
+          <t>[3.548219919204712, 8.691213607788086, 5.758365631103516, 6.487487316131592, 9.90291976928711, 6.694366455078125, 5.858821868896484]</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -1939,14 +1939,14 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>[8.691211386839777, 7.731836095243678, 8.609739822750038, 8.581772163170536, 8.94639168349315, 9.074630557371929, 9.319384200728924]</t>
+          <t>[8.691213607788086, 7.731835842132568, 8.609739303588867, 8.581768989562988, 8.94638442993164, 9.074629783630371, 9.31938362121582]</t>
         </is>
       </c>
       <c r="U16" t="n">
         <v>2</v>
       </c>
       <c r="V16" t="n">
-        <v>0.9216035148810561</v>
+        <v>0.9216032028198242</v>
       </c>
       <c r="W16" t="n">
         <v>0</v>
@@ -1955,7 +1955,7 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.155554</t>
+          <t>2025-10-17T02:10:07.600160</t>
         </is>
       </c>
     </row>
@@ -1978,7 +1978,7 @@
         <v>7</v>
       </c>
       <c r="F17" t="n">
-        <v>0.4762475941271153</v>
+        <v>0.476247085334295</v>
       </c>
       <c r="G17" t="n">
         <v>0.2857142857142857</v>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>[1.7238609439707153, 2.4434334544048664, 2.3008901008490206, 2.627912796286365, 2.2133899299550968, 2.550539891650585, 3.038968467681727]</t>
+          <t>[1.7238720655441284, 2.4434309005737305, 2.300889730453491, 2.6279022693634033, 2.213388204574585, 2.5505406856536865, 3.038969039916992]</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -2029,14 +2029,14 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>[1.7238609439707153, 2.3008901008490206, 2.2133899299550968, 2.4434334544048664, 2.627912796286365, 3.038968467681727, 6.031808407587342]</t>
+          <t>[1.7238720655441284, 2.300889730453491, 2.213388204574585, 2.4434309005737305, 2.6279022693634033, 3.038969039916992, 6.031808853149414]</t>
         </is>
       </c>
       <c r="U17" t="n">
         <v>2</v>
       </c>
       <c r="V17" t="n">
-        <v>0.5427547576736207</v>
+        <v>0.5427547693252563</v>
       </c>
       <c r="W17" t="n">
         <v>0</v>
@@ -2045,7 +2045,7 @@
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.155554</t>
+          <t>2025-10-17T02:10:07.601162</t>
         </is>
       </c>
     </row>
@@ -2068,7 +2068,7 @@
         <v>7</v>
       </c>
       <c r="F18" t="n">
-        <v>0.4762475941271153</v>
+        <v>0.476247085334295</v>
       </c>
       <c r="G18" t="n">
         <v>0.2857142857142857</v>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>[1.3550049834199527, 2.1108781737409203, 2.9421848739981007, 2.3781486454870766, 2.627912796286365, 2.9225667947525125, 3.353070551112966]</t>
+          <t>[1.3550022840499878, 2.110875129699707, 2.9421937465667725, 2.3781371116638184, 2.6279022693634033, 2.9225618839263916, 3.3530654907226562]</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -2119,14 +2119,14 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>[2.627912796286365, 2.796743980918212, 2.9225667947525125, 3.6776542059156947, 3.7257145542751764, 3.4966983271872256, 5.970870397142998]</t>
+          <t>[2.6279022693634033, 2.7967379093170166, 2.9225618839263916, 3.6776535511016846, 3.725713014602661, 3.496691942214966, 5.9708662033081055]</t>
         </is>
       </c>
       <c r="U18" t="n">
         <v>2</v>
       </c>
       <c r="V18" t="n">
-        <v>0.5590955779928345</v>
+        <v>0.5590962171554565</v>
       </c>
       <c r="W18" t="n">
         <v>0</v>
@@ -2135,7 +2135,7 @@
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.155554</t>
+          <t>2025-10-17T02:10:07.601162</t>
         </is>
       </c>
     </row>
@@ -2158,7 +2158,7 @@
         <v>7</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4762475941271153</v>
+        <v>0.476247085334295</v>
       </c>
       <c r="G19" t="n">
         <v>0.2857142857142857</v>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>[1.02730719349262, 2.3008901008490206, 2.0229240047329005, 2.9225667947525125, 3.8935267938311524, 3.228103787224398, 4.2501120677078585]</t>
+          <t>[1.0273101329803467, 2.300889730453491, 2.022925615310669, 2.9225618839263916, 3.8935210704803467, 3.228111982345581, 4.250108242034912]</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
@@ -2209,14 +2209,14 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>[1.02730719349262, 2.0229240047329005, 2.3008901008490206, 2.9225667947525125, 3.228103787224398, 3.639316011085586, 5.861988897205965]</t>
+          <t>[1.0273101329803467, 2.022925615310669, 2.300889730453491, 2.9225618839263916, 3.228111982345581, 3.639315605163574, 5.8619890213012695]</t>
         </is>
       </c>
       <c r="U19" t="n">
         <v>2</v>
       </c>
       <c r="V19" t="n">
-        <v>0.5870458256930585</v>
+        <v>0.5870458483695984</v>
       </c>
       <c r="W19" t="n">
         <v>0</v>
@@ -2225,7 +2225,7 @@
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.155554</t>
+          <t>2025-10-17T02:10:07.601162</t>
         </is>
       </c>
     </row>
@@ -2248,7 +2248,7 @@
         <v>7</v>
       </c>
       <c r="F20" t="n">
-        <v>0.4762475941271153</v>
+        <v>0.476247085334295</v>
       </c>
       <c r="G20" t="n">
         <v>0.2857142857142857</v>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>[1.270390163502212, 2.0229240047329005, 2.248409462917353, 2.2133899299550968, 2.7271522404792217, 2.1912232238840046, 2.4633435106922987]</t>
+          <t>[1.2703914642333984, 2.022925615310669, 2.2484099864959717, 2.213388204574585, 2.7271506786346436, 2.191220998764038, 2.463343381881714]</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
@@ -2299,14 +2299,14 @@
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>[2.0229240047329005, 2.2133899299550968, 2.248409462917353, 2.7271522404792217, 2.796743980918212, 3.5325657093384386, 5.384162362926166]</t>
+          <t>[2.022925615310669, 2.213388204574585, 2.2484099864959717, 2.7271506786346436, 2.7967379093170166, 3.532566547393799, 5.384163856506348]</t>
         </is>
       </c>
       <c r="U20" t="n">
         <v>2</v>
       </c>
       <c r="V20" t="n">
-        <v>0.53725349678003</v>
+        <v>0.5372540950775146</v>
       </c>
       <c r="W20" t="n">
         <v>0</v>
@@ -2315,7 +2315,7 @@
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.155554</t>
+          <t>2025-10-17T02:10:07.601162</t>
         </is>
       </c>
     </row>
@@ -2338,7 +2338,7 @@
         <v>7</v>
       </c>
       <c r="F21" t="n">
-        <v>0.4762475941271153</v>
+        <v>0.476247085334295</v>
       </c>
       <c r="G21" t="n">
         <v>0.2857142857142857</v>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>[8.691211386839777, 9.207417917519324, 8.894895806438829, 13.830842069171732, 10.461822702464078, 11.372812382036772, 9.74061119270624]</t>
+          <t>[8.691213607788086, 9.207416534423828, 8.894898414611816, 13.830842971801758, 10.461819648742676, 11.372812271118164, 9.74061107635498]</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
@@ -2389,14 +2389,14 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>[8.691211386839777, 9.828562976692579, 9.933644296013902, 10.808507914758495, 11.140759777554265, 11.009099614484562, 10.901504884982684]</t>
+          <t>[8.691213607788086, 9.828558921813965, 9.933645248413086, 10.808511734008789, 11.14076042175293, 11.009100914001465, 10.901507377624512]</t>
         </is>
       </c>
       <c r="U21" t="n">
         <v>2</v>
       </c>
       <c r="V21" t="n">
-        <v>1.256728913306704</v>
+        <v>1.256728887557983</v>
       </c>
       <c r="W21" t="n">
         <v>0</v>
@@ -2405,7 +2405,7 @@
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.155554</t>
+          <t>2025-10-17T02:10:07.601162</t>
         </is>
       </c>
     </row>
@@ -2428,7 +2428,7 @@
         <v>7</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4762475941271153</v>
+        <v>0.476247085334295</v>
       </c>
       <c r="G22" t="n">
         <v>0.2857142857142857</v>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>[1.02730719349262, 2.4434334544048664, 3.7905899556411646, 3.3227176388132555, 2.7271522404792217, 4.4170776760298525, 3.6776542059156947]</t>
+          <t>[1.0273101329803467, 2.4434309005737305, 3.7905890941619873, 3.322721242904663, 2.7271506786346436, 4.417076587677002, 3.6776535511016846]</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -2479,14 +2479,14 @@
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>[1.02730719349262, 2.4434334544048664, 2.7271522404792217, 3.3227176388132555, 3.6776542059156947, 3.930763646094779, 6.237906359894233]</t>
+          <t>[1.0273101329803467, 2.4434309005737305, 2.7271506786346436, 3.322721242904663, 3.6776535511016846, 3.9307637214660645, 6.2379069328308105]</t>
         </is>
       </c>
       <c r="U22" t="n">
         <v>2</v>
       </c>
       <c r="V22" t="n">
-        <v>0.6351716245864483</v>
+        <v>0.6351715326309204</v>
       </c>
       <c r="W22" t="n">
         <v>0</v>
@@ -2495,7 +2495,7 @@
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.156569</t>
+          <t>2025-10-17T02:10:07.602160</t>
         </is>
       </c>
     </row>
@@ -2518,7 +2518,7 @@
         <v>7</v>
       </c>
       <c r="F23" t="n">
-        <v>0.4762475941271153</v>
+        <v>0.476247085334295</v>
       </c>
       <c r="G23" t="n">
         <v>0.2857142857142857</v>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>[3.9940960660638245, 3.6129325646687236, 3.9857840791532855, 3.5137164996797625, 3.133360360859858, 3.772018568783384, 8.738918927498052]</t>
+          <t>[3.9940896034240723, 3.612931966781616, 3.9857804775238037, 3.513723611831665, 3.133359909057617, 3.7720181941986084, 8.738912582397461]</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
@@ -2569,14 +2569,14 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>[3.6129325646687236, 5.384162362926166, 5.861988897205965, 5.970870397142998, 6.016938439507509, 6.031808407587342, 6.237906359894233]</t>
+          <t>[3.612931966781616, 5.384163856506348, 5.8619890213012695, 5.9708662033081055, 6.016942501068115, 6.031808853149414, 6.2379069328308105]</t>
         </is>
       </c>
       <c r="U23" t="n">
         <v>2</v>
       </c>
       <c r="V23" t="n">
-        <v>0.8878564287652138</v>
+        <v>0.887856125831604</v>
       </c>
       <c r="W23" t="n">
         <v>0</v>
@@ -2585,7 +2585,7 @@
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.156569</t>
+          <t>2025-10-17T02:10:07.602160</t>
         </is>
       </c>
     </row>
@@ -2608,7 +2608,7 @@
         <v>7</v>
       </c>
       <c r="F24" t="n">
-        <v>0.4762475941271153</v>
+        <v>0.476247085334295</v>
       </c>
       <c r="G24" t="n">
         <v>0.2857142857142857</v>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>[3.3579545061816214, 3.038968467681727, 3.6129325646687236, 3.092282199641918, 2.8238881125594335, 3.4966983271872256, 3.930763646094779]</t>
+          <t>[3.3579466342926025, 3.038969039916992, 3.612931966781616, 3.0922813415527344, 2.8238894939422607, 3.496691942214966, 3.9307637214660645]</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
@@ -2659,14 +2659,14 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>[3.038968467681727, 3.4966983271872256, 3.6129325646687236, 3.639316011085586, 3.6992423534262557, 3.5325657093384386, 3.930763646094779]</t>
+          <t>[3.038969039916992, 3.496691942214966, 3.612931966781616, 3.639315605163574, 3.699251413345337, 3.532566547393799, 3.9307637214660645]</t>
         </is>
       </c>
       <c r="U24" t="n">
         <v>2</v>
       </c>
       <c r="V24" t="n">
-        <v>0.9351432253651912</v>
+        <v>0.9351437091827393</v>
       </c>
       <c r="W24" t="n">
         <v>0</v>
@@ -2675,7 +2675,7 @@
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.156569</t>
+          <t>2025-10-17T02:10:07.602160</t>
         </is>
       </c>
     </row>
@@ -2698,7 +2698,7 @@
         <v>7</v>
       </c>
       <c r="F25" t="n">
-        <v>0.4762475941271153</v>
+        <v>0.476247085334295</v>
       </c>
       <c r="G25" t="n">
         <v>0.2857142857142857</v>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>[1.7238609439707153, 2.248409462917353, 3.682756134418453, 3.3227176388132555, 2.847716027962298, 3.228103787224398, 3.1367684717948636]</t>
+          <t>[1.7238720655441284, 2.2484099864959717, 3.682757616043091, 3.322721242904663, 2.8477210998535156, 3.228111982345581, 3.136768102645874]</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
@@ -2749,14 +2749,14 @@
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>[1.7238609439707153, 2.248409462917353, 3.3227176388132555, 3.228103787224398, 3.7257145542751764, 3.6992423534262557, 6.016938439507509]</t>
+          <t>[1.7238720655441284, 2.2484099864959717, 3.322721242904663, 3.228111982345581, 3.725713014602661, 3.699251413345337, 6.016942501068115]</t>
         </is>
       </c>
       <c r="U25" t="n">
         <v>2</v>
       </c>
       <c r="V25" t="n">
-        <v>0.6654737504131258</v>
+        <v>0.6654731035232544</v>
       </c>
       <c r="W25" t="n">
         <v>0</v>
@@ -2765,7 +2765,7 @@
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.156569</t>
+          <t>2025-10-17T02:10:07.602160</t>
         </is>
       </c>
     </row>
@@ -2788,7 +2788,7 @@
         <v>7</v>
       </c>
       <c r="F26" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G26" t="n">
         <v>0.2857142857142857</v>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>[3.682756134418453, 5.021605002625455, 4.70630304597658, 9.207417917519324, 5.405719067891872, 8.388981090374504, 7.5877058337289265]</t>
+          <t>[3.682757616043091, 5.021600246429443, 4.706303119659424, 9.207416534423828, 5.405718803405762, 8.388983726501465, 7.5876994132995605]</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
@@ -2839,14 +2839,14 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>[6.08800436829768, 7.964256258235821, 8.471146633002151, 7.782585844233039, 5.95449152616891, 9.602741008279496, 6.843429901519849]</t>
+          <t>[6.087997913360596, 7.964256763458252, 8.471141815185547, 7.782583713531494, 5.954493045806885, 9.602742195129395, 6.843430519104004]</t>
         </is>
       </c>
       <c r="U26" t="n">
         <v>2</v>
       </c>
       <c r="V26" t="n">
-        <v>1.090825944952199</v>
+        <v>1.090826153755188</v>
       </c>
       <c r="W26" t="n">
         <v>1</v>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.241951</t>
+          <t>2025-10-17T02:10:07.708207</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
         <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G27" t="n">
         <v>0.2857142857142857</v>
@@ -2923,7 +2923,7 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>[0.8132081400250286, 1.5868689295900902, 1.5875982496431946, 1.4858066535973735, 1.6002348222769218, 1.922422725330582, 1.6309597213366673]</t>
+          <t>[0.8132038116455078, 1.586868405342102, 1.5875941514968872, 1.4857956171035767, 1.6002230644226074, 1.9224257469177246, 1.6309336423873901]</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
@@ -2933,14 +2933,14 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>[3.809058612177697, 3.489683763572442, 6.08800436829768, 5.247392155625091, 5.183228044239134, 4.850350457556759, 7.007670571360432]</t>
+          <t>[3.809053421020508, 3.489682912826538, 6.087997913360596, 5.247391700744629, 5.183218955993652, 4.85034704208374, 7.00767183303833]</t>
         </is>
       </c>
       <c r="U27" t="n">
         <v>2</v>
       </c>
       <c r="V27" t="n">
-        <v>0.5878918847498597</v>
+        <v>0.587891697883606</v>
       </c>
       <c r="W27" t="n">
         <v>3</v>
@@ -2953,7 +2953,7 @@
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.242967</t>
+          <t>2025-10-17T02:10:07.708207</t>
         </is>
       </c>
     </row>
@@ -2976,7 +2976,7 @@
         <v>7</v>
       </c>
       <c r="F28" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G28" t="n">
         <v>0.2857142857142857</v>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>[0.6938538718042702, 0.7095152903098895, 1.2714170344520064, 1.5296665982953364, 1.32061194669919, 1.1889773334939922, 1.4472985267768135]</t>
+          <t>[0.6938520073890686, 0.7095147371292114, 1.2714117765426636, 1.5296647548675537, 1.3206110000610352, 1.1889803409576416, 1.4472988843917847]</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -3027,14 +3027,14 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>[0.6938538718042702, 0.7095152903098895, 1.2714170344520064, 1.5296665982953364, 1.32061194669919, 1.1889773334939922, 1.4472985267768135]</t>
+          <t>[0.6938520073890686, 0.7095147371292114, 1.2714117765426636, 1.5296647548675537, 1.3206110000610352, 1.1889803409576416, 1.4472988843917847]</t>
         </is>
       </c>
       <c r="U28" t="n">
         <v>2</v>
       </c>
       <c r="V28" t="n">
-        <v>0.6609103897926523</v>
+        <v>0.6609089970588684</v>
       </c>
       <c r="W28" t="n">
         <v>1</v>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.243642</t>
+          <t>2025-10-17T02:10:07.709202</t>
         </is>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
         <v>7</v>
       </c>
       <c r="F29" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G29" t="n">
         <v>0.2857142857142857</v>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>[1.1962071176531426, 1.4052520928097405, 1.5114443168656573, 1.5090353997195989, 1.5793456969697512, 1.7265879571947085, 2.767818741427769]</t>
+          <t>[1.1962192058563232, 1.4052584171295166, 1.5114425420761108, 1.5090450048446655, 1.5793581008911133, 1.7265819311141968, 2.7678287029266357]</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
@@ -3121,14 +3121,14 @@
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>[1.1962071176531426, 1.4052520928097405, 1.5114443168656573, 1.5090353997195989, 1.5793456969697512, 1.7265879571947085, 2.767818741427769]</t>
+          <t>[1.1962192058563232, 1.4052584171295166, 1.5114425420761108, 1.5090450048446655, 1.5793581008911133, 1.7265819311141968, 2.7678287029266357]</t>
         </is>
       </c>
       <c r="U29" t="n">
         <v>2</v>
       </c>
       <c r="V29" t="n">
-        <v>0.6468385413566489</v>
+        <v>0.6468383073806763</v>
       </c>
       <c r="W29" t="n">
         <v>2</v>
@@ -3141,7 +3141,7 @@
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.244156</t>
+          <t>2025-10-17T02:10:07.709202</t>
         </is>
       </c>
     </row>
@@ -3164,7 +3164,7 @@
         <v>7</v>
       </c>
       <c r="F30" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G30" t="n">
         <v>0.2857142857142857</v>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>[0.5247670678089587, 1.0627897260130672, 1.0365164925602255, 1.0264295246425166, 1.0427116849041143, 1.2714170344520064, 1.5825925572439319]</t>
+          <t>[0.5247544646263123, 1.0627883672714233, 1.0364985466003418, 1.026412844657898, 1.042699933052063, 1.2714117765426636, 1.5825912952423096]</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -3215,14 +3215,14 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>[0.5247670678089587, 1.0627897260130672, 1.0365164925602255, 1.0264295246425166, 1.0427116849041143, 1.2714170344520064, 1.5825925572439319]</t>
+          <t>[0.5247544646263123, 1.0627883672714233, 1.0364985466003418, 1.026412844657898, 1.042699933052063, 1.2714117765426636, 1.5825912952423096]</t>
         </is>
       </c>
       <c r="U30" t="n">
         <v>2</v>
       </c>
       <c r="V30" t="n">
-        <v>0.6342503428067964</v>
+        <v>0.6342445611953735</v>
       </c>
       <c r="W30" t="n">
         <v>0</v>
@@ -3231,7 +3231,7 @@
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.244156</t>
+          <t>2025-10-17T02:10:07.709202</t>
         </is>
       </c>
     </row>
@@ -3254,7 +3254,7 @@
         <v>7</v>
       </c>
       <c r="F31" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G31" t="n">
         <v>0.2857142857142857</v>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>[0.5955520820772918, 0.7853120750288224, 1.0365164925602255, 1.1688040592017273, 1.32061194669919, 1.215666646680279, 1.6141646739074402]</t>
+          <t>[0.5955532789230347, 0.7853057980537415, 1.0364985466003418, 1.1688058376312256, 1.3206110000610352, 1.215668797492981, 1.6141602993011475]</t>
         </is>
       </c>
       <c r="S31" t="inlineStr">
@@ -3305,14 +3305,14 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>[0.5955520820772918, 0.7853120750288224, 1.0365164925602255, 1.1688040592017273, 1.32061194669919, 1.215666646680279, 1.6141646739074402]</t>
+          <t>[0.5955532789230347, 0.7853057980537415, 1.0364985466003418, 1.1688058376312256, 1.3206110000610352, 1.215668797492981, 1.6141602993011475]</t>
         </is>
       </c>
       <c r="U31" t="n">
         <v>2</v>
       </c>
       <c r="V31" t="n">
-        <v>0.5639605563306247</v>
+        <v>0.5639538764953613</v>
       </c>
       <c r="W31" t="n">
         <v>1</v>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.244156</t>
+          <t>2025-10-17T02:10:07.709202</t>
         </is>
       </c>
     </row>
@@ -3348,7 +3348,7 @@
         <v>7</v>
       </c>
       <c r="F32" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G32" t="n">
         <v>0.2857142857142857</v>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>[4.05470661044856, 2.8743801847924346, 3.5498127594816147, 4.931710867209231, 3.9400554781817645, 3.491143442024662, 4.050657684538021]</t>
+          <t>[4.054708003997803, 2.8743762969970703, 3.549809217453003, 4.931705474853516, 3.940061569213867, 3.491143226623535, 4.050656318664551]</t>
         </is>
       </c>
       <c r="S32" t="inlineStr">
@@ -3399,14 +3399,14 @@
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t>[3.809058612177697, 4.05470661044856, 4.931710867209231, 4.900343505852515, 8.471146633002151, 5.014385606825274, 5.74133915986708]</t>
+          <t>[3.809053421020508, 4.054708003997803, 4.931705474853516, 4.90034294128418, 8.471141815185547, 5.014385223388672, 5.741334438323975]</t>
         </is>
       </c>
       <c r="U32" t="n">
         <v>2</v>
       </c>
       <c r="V32" t="n">
-        <v>0.9614203639120933</v>
+        <v>0.9614191055297852</v>
       </c>
       <c r="W32" t="n">
         <v>0</v>
@@ -3415,7 +3415,7 @@
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.244156</t>
+          <t>2025-10-17T02:10:07.709202</t>
         </is>
       </c>
     </row>
@@ -3438,7 +3438,7 @@
         <v>7</v>
       </c>
       <c r="F33" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G33" t="n">
         <v>0.2857142857142857</v>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>[0.5768095704933661, 0.5955520820772918, 1.0627897260130672, 1.1515591686123146, 1.4561485338614213, 1.6920400399297932, 1.8567672404495317]</t>
+          <t>[0.5768178105354309, 0.5955532789230347, 1.0627883672714233, 1.151566743850708, 1.4561500549316406, 1.6920398473739624, 1.856772780418396]</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
@@ -3489,14 +3489,14 @@
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>[0.5768095704933661, 0.5955520820772918, 1.0627897260130672, 1.1515591686123146, 1.4561485338614213, 1.6920400399297932, 1.8567672404495317]</t>
+          <t>[0.5768178105354309, 0.5955532789230347, 1.0627883672714233, 1.151566743850708, 1.4561500549316406, 1.6920398473739624, 1.856772780418396]</t>
         </is>
       </c>
       <c r="U33" t="n">
         <v>2</v>
       </c>
       <c r="V33" t="n">
-        <v>0.4819979777883111</v>
+        <v>0.481997549533844</v>
       </c>
       <c r="W33" t="n">
         <v>3</v>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.244156</t>
+          <t>2025-10-17T02:10:07.710203</t>
         </is>
       </c>
     </row>
@@ -3532,7 +3532,7 @@
         <v>7</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G34" t="n">
         <v>0.2857142857142857</v>
@@ -3573,7 +3573,7 @@
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>[0.9638482758194614, 1.0427116849041143, 1.1515591686123146, 1.2844867596432914, 1.1688040592017273, 1.1889773334939922, 1.2921742063603394]</t>
+          <t>[0.963847815990448, 1.042699933052063, 1.151566743850708, 1.2844855785369873, 1.1688058376312256, 1.1889803409576416, 1.2921749353408813]</t>
         </is>
       </c>
       <c r="S34" t="inlineStr">
@@ -3583,14 +3583,14 @@
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t>[0.9638482758194614, 1.0427116849041143, 1.1515591686123146, 1.2844867596432914, 1.1688040592017273, 1.1889773334939922, 1.2921742063603394]</t>
+          <t>[0.963847815990448, 1.042699933052063, 1.151566743850708, 1.2844855785369873, 1.1688058376312256, 1.1889803409576416, 1.2921749353408813]</t>
         </is>
       </c>
       <c r="U34" t="n">
         <v>2</v>
       </c>
       <c r="V34" t="n">
-        <v>0.7362978162648894</v>
+        <v>0.7362955212593079</v>
       </c>
       <c r="W34" t="n">
         <v>1</v>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.245176</t>
+          <t>2025-10-17T02:10:07.710203</t>
         </is>
       </c>
     </row>
@@ -3626,7 +3626,7 @@
         <v>7</v>
       </c>
       <c r="F35" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G35" t="n">
         <v>0.2857142857142857</v>
@@ -3667,7 +3667,7 @@
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>[0.6938538718042702, 1.232152903578428, 1.2844867596432914, 1.5825925572439319, 1.6141646739074402, 1.972033621587465, 1.7865657354714215]</t>
+          <t>[0.6938520073890686, 1.2321480512619019, 1.2844855785369873, 1.5825912952423096, 1.6141602993011475, 1.9720324277877808, 1.7865649461746216]</t>
         </is>
       </c>
       <c r="S35" t="inlineStr">
@@ -3677,14 +3677,14 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>[0.6938538718042702, 1.232152903578428, 1.2844867596432914, 1.5825925572439319, 1.6141646739074402, 1.972033621587465, 1.7865657354714215]</t>
+          <t>[0.6938520073890686, 1.2321480512619019, 1.2844855785369873, 1.5825912952423096, 1.6141602993011475, 1.9720324277877808, 1.7865649461746216]</t>
         </is>
       </c>
       <c r="U35" t="n">
         <v>2</v>
       </c>
       <c r="V35" t="n">
-        <v>0.7882670078345039</v>
+        <v>0.7882651090621948</v>
       </c>
       <c r="W35" t="n">
         <v>1</v>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.245176</t>
+          <t>2025-10-17T02:10:07.710203</t>
         </is>
       </c>
     </row>
@@ -3720,7 +3720,7 @@
         <v>7</v>
       </c>
       <c r="F36" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G36" t="n">
         <v>0.2857142857142857</v>
@@ -3761,7 +3761,7 @@
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>[2.2655902011080813, 2.009402944755667, 2.3744285735325943, 2.069902236630937, 2.1498598411769523, 2.1959409717746525, 2.6336450736208743]</t>
+          <t>[2.265591859817505, 2.0094025135040283, 2.374429702758789, 2.0699026584625244, 2.1498682498931885, 2.195941925048828, 2.633648633956909]</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
@@ -3771,14 +3771,14 @@
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>[2.2655902011080813, 3.489683763572442, 2.009402944755667, 2.3744285735325943, 2.069902236630937, 2.1959409717746525, 2.4429403769269977]</t>
+          <t>[2.265591859817505, 3.489682912826538, 2.0094025135040283, 2.374429702758789, 2.0699026584625244, 2.195941925048828, 2.442943572998047]</t>
         </is>
       </c>
       <c r="U36" t="n">
         <v>2</v>
       </c>
       <c r="V36" t="n">
-        <v>1.053198726969512</v>
+        <v>1.053199052810669</v>
       </c>
       <c r="W36" t="n">
         <v>0</v>
@@ -3787,7 +3787,7 @@
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.245176</t>
+          <t>2025-10-17T02:10:07.710203</t>
         </is>
       </c>
     </row>
@@ -3810,7 +3810,7 @@
         <v>7</v>
       </c>
       <c r="F37" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G37" t="n">
         <v>0.2857142857142857</v>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>[0.554208474292604, 0.9788096610379503, 1.1962071176531426, 1.15532112645773, 1.1788478002932243, 1.196821520219185, 2.3023860235789515]</t>
+          <t>[0.5542061924934387, 0.9788116216659546, 1.1962192058563232, 1.1553232669830322, 1.1788504123687744, 1.1968179941177368, 2.302386522293091]</t>
         </is>
       </c>
       <c r="S37" t="inlineStr">
@@ -3861,14 +3861,14 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>[0.554208474292604, 0.9788096610379503, 1.1962071176531426, 1.15532112645773, 1.1788478002932243, 1.196821520219185, 2.3023860235789515]</t>
+          <t>[0.5542061924934387, 0.9788116216659546, 1.1962192058563232, 1.1553232669830322, 1.1788504123687744, 1.1968179941177368, 2.302386522293091]</t>
         </is>
       </c>
       <c r="U37" t="n">
         <v>2</v>
       </c>
       <c r="V37" t="n">
-        <v>0.4933542131734344</v>
+        <v>0.4933568239212036</v>
       </c>
       <c r="W37" t="n">
         <v>3</v>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.245176</t>
+          <t>2025-10-17T02:10:07.710203</t>
         </is>
       </c>
     </row>
@@ -3904,7 +3904,7 @@
         <v>7</v>
       </c>
       <c r="F38" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G38" t="n">
         <v>0.2857142857142857</v>
@@ -3945,7 +3945,7 @@
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>[4.337198191692961, 4.05470661044856, 6.487488755518677, 5.440198495444032, 8.820757032771018, 5.109254203889771, 4.391370694579391]</t>
+          <t>[4.337198257446289, 4.054708003997803, 6.487487316131592, 5.44020938873291, 8.82075309753418, 5.109254360198975, 4.3913702964782715]</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
@@ -3955,14 +3955,14 @@
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>[4.05470661044856, 4.337198191692961, 5.247392155625091, 5.440198495444032, 4.391370694579391, 4.788558760473677, 4.678288879544833]</t>
+          <t>[4.054708003997803, 4.337198257446289, 5.247391700744629, 5.44020938873291, 4.3913702964782715, 4.788558006286621, 4.678295612335205]</t>
         </is>
       </c>
       <c r="U38" t="n">
         <v>2</v>
       </c>
       <c r="V38" t="n">
-        <v>1.074541284086465</v>
+        <v>1.074542284011841</v>
       </c>
       <c r="W38" t="n">
         <v>0</v>
@@ -3971,7 +3971,7 @@
       <c r="Y38" t="inlineStr"/>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.245907</t>
+          <t>2025-10-17T02:10:07.711201</t>
         </is>
       </c>
     </row>
@@ -3994,7 +3994,7 @@
         <v>7</v>
       </c>
       <c r="F39" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G39" t="n">
         <v>0.2857142857142857</v>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>[4.087903692704581, 5.758371013344655, 3.762171276613728, 3.718255724775455, 5.440198495444032, 3.8400893679327046, 3.842576423535419]</t>
+          <t>[4.087904453277588, 5.758365631103516, 3.762176036834717, 3.718254804611206, 5.44020938873291, 3.840088129043579, 3.842573881149292]</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
@@ -4045,14 +4045,14 @@
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>[4.087903692704581, 3.762171276613728, 5.440198495444032, 3.718255724775455, 3.8400893679327046, 3.842576423535419, 3.7610177832708014]</t>
+          <t>[4.087904453277588, 3.762176036834717, 5.44020938873291, 3.718254804611206, 3.840088129043579, 3.842573881149292, 3.7610156536102295]</t>
         </is>
       </c>
       <c r="U39" t="n">
         <v>2</v>
       </c>
       <c r="V39" t="n">
-        <v>1.150547519374437</v>
+        <v>1.150546550750732</v>
       </c>
       <c r="W39" t="n">
         <v>0</v>
@@ -4061,7 +4061,7 @@
       <c r="Y39" t="inlineStr"/>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.245907</t>
+          <t>2025-10-17T02:10:07.711201</t>
         </is>
       </c>
     </row>
@@ -4084,7 +4084,7 @@
         <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G40" t="n">
         <v>0.2857142857142857</v>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>[0.5247670678089587, 0.5768095704933661, 0.7853120750288224, 0.9638482758194614, 1.1512872277874546, 1.4472985267768135, 1.6623535242660015]</t>
+          <t>[0.5247544646263123, 0.5768178105354309, 0.7853057980537415, 0.963847815990448, 1.1512864828109741, 1.4472988843917847, 1.6623544692993164]</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
@@ -4135,14 +4135,14 @@
       </c>
       <c r="T40" t="inlineStr">
         <is>
-          <t>[0.5247670678089587, 0.5768095704933661, 0.7853120750288224, 0.9638482758194614, 1.1512872277874546, 1.4472985267768135, 1.6623535242660015]</t>
+          <t>[0.5247544646263123, 0.5768178105354309, 0.7853057980537415, 0.963847815990448, 1.1512864828109741, 1.4472988843917847, 1.6623544692993164]</t>
         </is>
       </c>
       <c r="U40" t="n">
         <v>2</v>
       </c>
       <c r="V40" t="n">
-        <v>0.4038627578739663</v>
+        <v>0.4038631319999695</v>
       </c>
       <c r="W40" t="n">
         <v>2</v>
@@ -4155,7 +4155,7 @@
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.245907</t>
+          <t>2025-10-17T02:10:07.711201</t>
         </is>
       </c>
     </row>
@@ -4178,7 +4178,7 @@
         <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G41" t="n">
         <v>0.2857142857142857</v>
@@ -4219,7 +4219,7 @@
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>[3.548220758848561, 4.337198191692961, 4.087903692704581, 4.931710867209231, 8.894895806438829, 4.539073032076113, 4.718257125202034]</t>
+          <t>[3.548219919204712, 4.337198257446289, 4.087904453277588, 4.931705474853516, 8.894898414611816, 4.53907585144043, 4.718254566192627]</t>
         </is>
       </c>
       <c r="S41" t="inlineStr">
@@ -4229,14 +4229,14 @@
       </c>
       <c r="T41" t="inlineStr">
         <is>
-          <t>[4.337198191692961, 4.087903692704581, 4.931710867209231, 5.183228044239134, 4.539073032076113, 4.718257125202034, 4.522115957094709]</t>
+          <t>[4.337198257446289, 4.087904453277588, 4.931705474853516, 5.183218955993652, 4.53907585144043, 4.718254566192627, 4.522115707397461]</t>
         </is>
       </c>
       <c r="U41" t="n">
         <v>2</v>
       </c>
       <c r="V41" t="n">
-        <v>0.9351363228820693</v>
+        <v>0.9351364374160767</v>
       </c>
       <c r="W41" t="n">
         <v>0</v>
@@ -4245,7 +4245,7 @@
       <c r="Y41" t="inlineStr"/>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.246418</t>
+          <t>2025-10-17T02:10:07.711201</t>
         </is>
       </c>
     </row>
@@ -4268,7 +4268,7 @@
         <v>7</v>
       </c>
       <c r="F42" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G42" t="n">
         <v>0.2857142857142857</v>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>[0.4555300636353425, 0.5437260897988515, 0.8630496944521113, 0.9788096610379503, 0.9866147171205542, 1.5090353997195989, 1.987839538370493]</t>
+          <t>[0.4555348753929138, 0.5437226295471191, 0.8630491495132446, 0.9788116216659546, 0.9866169691085815, 1.5090450048446655, 1.987839698791504]</t>
         </is>
       </c>
       <c r="S42" t="inlineStr">
@@ -4319,14 +4319,14 @@
       </c>
       <c r="T42" t="inlineStr">
         <is>
-          <t>[0.4555300636353425, 0.5437260897988515, 0.8630496944521113, 0.9788096610379503, 0.9866147171205542, 1.5090353997195989, 1.987839538370493]</t>
+          <t>[0.4555348753929138, 0.5437226295471191, 0.8630491495132446, 0.9788116216659546, 0.9866169691085815, 1.5090450048446655, 1.987839698791504]</t>
         </is>
       </c>
       <c r="U42" t="n">
         <v>2</v>
       </c>
       <c r="V42" t="n">
-        <v>0.3561481351826532</v>
+        <v>0.3561474978923798</v>
       </c>
       <c r="W42" t="n">
         <v>1</v>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.246418</t>
+          <t>2025-10-17T02:10:07.711201</t>
         </is>
       </c>
     </row>
@@ -4362,7 +4362,7 @@
         <v>7</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G43" t="n">
         <v>0.2857142857142857</v>
@@ -4403,7 +4403,7 @@
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>[0.8630496944521113, 0.9548645626090493, 1.15532112645773, 1.0304942909300825, 1.2386401795972093, 1.5793456969697512, 2.4712924331226453]</t>
+          <t>[0.8630491495132446, 0.9548653364181519, 1.1553232669830322, 1.0304895639419556, 1.2386415004730225, 1.5793581008911133, 2.4712913036346436]</t>
         </is>
       </c>
       <c r="S43" t="inlineStr">
@@ -4413,14 +4413,14 @@
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t>[0.8630496944521113, 0.9548645626090493, 1.15532112645773, 1.0304942909300825, 1.2386401795972093, 1.5793456969697512, 2.4712924331226453]</t>
+          <t>[0.8630491495132446, 0.9548653364181519, 1.1553232669830322, 1.0304895639419556, 1.2386415004730225, 1.5793581008911133, 2.4712913036346436]</t>
         </is>
       </c>
       <c r="U43" t="n">
         <v>2</v>
       </c>
       <c r="V43" t="n">
-        <v>0.492971664196956</v>
+        <v>0.4929726719856262</v>
       </c>
       <c r="W43" t="n">
         <v>0</v>
@@ -4429,7 +4429,7 @@
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.246418</t>
+          <t>2025-10-17T02:10:07.711201</t>
         </is>
       </c>
     </row>
@@ -4452,7 +4452,7 @@
         <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G44" t="n">
         <v>0.2857142857142857</v>
@@ -4493,7 +4493,7 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>[1.2254670342423102, 1.5296665982953364, 1.972033621587465, 1.7913607550454447, 2.3023860235789515, 2.007189037033557, 2.4712924331226453]</t>
+          <t>[1.225460410118103, 1.5296647548675537, 1.9720324277877808, 1.7913583517074585, 2.302386522293091, 2.007189989089966, 2.4712913036346436]</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
@@ -4503,14 +4503,14 @@
       </c>
       <c r="T44" t="inlineStr">
         <is>
-          <t>[1.2254670342423102, 1.5296665982953364, 1.972033621587465, 1.7913607550454447, 2.3023860235789515, 2.007189037033557, 2.4712924331226453]</t>
+          <t>[1.225460410118103, 1.5296647548675537, 1.9720324277877808, 1.7913583517074585, 2.302386522293091, 2.007189989089966, 2.4712913036346436]</t>
         </is>
       </c>
       <c r="U44" t="n">
         <v>2</v>
       </c>
       <c r="V44" t="n">
-        <v>0.8767747868883247</v>
+        <v>0.8767750263214111</v>
       </c>
       <c r="W44" t="n">
         <v>1</v>
@@ -4523,7 +4523,7 @@
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.246418</t>
+          <t>2025-10-17T02:10:07.712200</t>
         </is>
       </c>
     </row>
@@ -4546,7 +4546,7 @@
         <v>7</v>
       </c>
       <c r="F45" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G45" t="n">
         <v>0.2857142857142857</v>
@@ -4587,7 +4587,7 @@
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>[0.554208474292604, 0.9866147171205542, 1.1374318846972276, 1.0372642603783018, 1.2386401795972093, 1.4052520928097405, 2.2655902011080813]</t>
+          <t>[0.5542061924934387, 0.9866169691085815, 1.1374363899230957, 1.0372637510299683, 1.2386415004730225, 1.4052584171295166, 2.265591859817505]</t>
         </is>
       </c>
       <c r="S45" t="inlineStr">
@@ -4597,14 +4597,14 @@
       </c>
       <c r="T45" t="inlineStr">
         <is>
-          <t>[0.554208474292604, 0.9866147171205542, 1.1374318846972276, 1.0372642603783018, 1.2386401795972093, 1.4052520928097405, 2.2655902011080813]</t>
+          <t>[0.5542061924934387, 0.9866169691085815, 1.1374363899230957, 1.0372637510299683, 1.2386415004730225, 1.4052584171295166, 2.265591859817505]</t>
         </is>
       </c>
       <c r="U45" t="n">
         <v>2</v>
       </c>
       <c r="V45" t="n">
-        <v>0.5129431377389692</v>
+        <v>0.5129446983337402</v>
       </c>
       <c r="W45" t="n">
         <v>2</v>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.246418</t>
+          <t>2025-10-17T02:10:07.712200</t>
         </is>
       </c>
     </row>
@@ -4640,7 +4640,7 @@
         <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G46" t="n">
         <v>0.2857142857142857</v>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>[0.4956847553434702, 0.5437260897988515, 1.0304942909300825, 1.0372642603783018, 1.196821520219185, 1.7265879571947085, 1.6623535242660015]</t>
+          <t>[0.49568384885787964, 0.5437226295471191, 1.0304895639419556, 1.0372637510299683, 1.1968179941177368, 1.7265819311141968, 1.6623544692993164]</t>
         </is>
       </c>
       <c r="S46" t="inlineStr">
@@ -4691,14 +4691,14 @@
       </c>
       <c r="T46" t="inlineStr">
         <is>
-          <t>[0.4956847553434702, 0.5437260897988515, 1.0304942909300825, 1.0372642603783018, 1.196821520219185, 1.7265879571947085, 1.6623535242660015]</t>
+          <t>[0.49568384885787964, 0.5437226295471191, 1.0304895639419556, 1.0372637510299683, 1.1968179941177368, 1.7265819311141968, 1.6623544692993164]</t>
         </is>
       </c>
       <c r="U46" t="n">
         <v>2</v>
       </c>
       <c r="V46" t="n">
-        <v>0.4150254282318591</v>
+        <v>0.4150242209434509</v>
       </c>
       <c r="W46" t="n">
         <v>2</v>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.246418</t>
+          <t>2025-10-17T02:10:07.712200</t>
         </is>
       </c>
     </row>
@@ -4734,7 +4734,7 @@
         <v>7</v>
       </c>
       <c r="F47" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G47" t="n">
         <v>0.2857142857142857</v>
@@ -4775,7 +4775,7 @@
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>[0.4555300636353425, 0.4956847553434702, 0.9548645626090493, 1.1374318846972276, 1.1788478002932243, 1.5114443168656573, 2.0850346828531623]</t>
+          <t>[0.4555348753929138, 0.49568384885787964, 0.9548653364181519, 1.1374363899230957, 1.1788504123687744, 1.5114425420761108, 2.0850367546081543]</t>
         </is>
       </c>
       <c r="S47" t="inlineStr">
@@ -4785,14 +4785,14 @@
       </c>
       <c r="T47" t="inlineStr">
         <is>
-          <t>[0.4555300636353425, 0.4956847553434702, 0.9548645626090493, 1.1374318846972276, 1.1788478002932243, 1.5114443168656573, 2.4429403769269977]</t>
+          <t>[0.4555348753929138, 0.49568384885787964, 0.9548653364181519, 1.1374363899230957, 1.1788504123687744, 1.5114425420761108, 2.442943572998047]</t>
         </is>
       </c>
       <c r="U47" t="n">
         <v>2</v>
       </c>
       <c r="V47" t="n">
-        <v>0.3568397283959914</v>
+        <v>0.3568399250507355</v>
       </c>
       <c r="W47" t="n">
         <v>0</v>
@@ -4801,7 +4801,7 @@
       <c r="Y47" t="inlineStr"/>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.247403</t>
+          <t>2025-10-17T02:10:07.712200</t>
         </is>
       </c>
     </row>
@@ -4824,7 +4824,7 @@
         <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>0.5844642634891221</v>
+        <v>0.5844655394036213</v>
       </c>
       <c r="G48" t="n">
         <v>0.2857142857142857</v>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>[0.7095152903098895, 1.2254670342423102, 1.0264295246425166, 1.232152903578428, 1.1512872277874546, 1.215666646680279, 1.4561485338614213]</t>
+          <t>[0.7095147371292114, 1.225460410118103, 1.026412844657898, 1.2321480512619019, 1.1512864828109741, 1.215668797492981, 1.4561500549316406]</t>
         </is>
       </c>
       <c r="S48" t="inlineStr">
@@ -4875,14 +4875,14 @@
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t>[0.7095152903098895, 1.2254670342423102, 1.0264295246425166, 1.232152903578428, 1.1512872277874546, 1.215666646680279, 1.4561485338614213]</t>
+          <t>[0.7095147371292114, 1.225460410118103, 1.026412844657898, 1.2321480512619019, 1.1512864828109741, 1.215668797492981, 1.4561500549316406]</t>
         </is>
       </c>
       <c r="U48" t="n">
         <v>2</v>
       </c>
       <c r="V48" t="n">
-        <v>0.7167712447983688</v>
+        <v>0.7167636752128601</v>
       </c>
       <c r="W48" t="n">
         <v>1</v>
@@ -4895,7 +4895,7 @@
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>2025-10-16T12:16:25.247403</t>
+          <t>2025-10-17T02:10:07.712200</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
mas cambios sobre lanotebook
tardo 60 min, demasiado. El mejor tiempo fue 20 min
</commit_message>
<xml_diff>
--- a/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_glass_D25_R25_Pentropia.xlsx
+++ b/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_glass_D25_R25_Pentropia.xlsx
@@ -651,7 +651,7 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.542671</t>
+          <t>2025-10-17T07:09:26.023691</t>
         </is>
       </c>
     </row>
@@ -745,7 +745,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.543667</t>
+          <t>2025-10-17T07:09:26.023691</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.543667</t>
+          <t>2025-10-17T07:09:26.023691</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.543667</t>
+          <t>2025-10-17T07:09:26.023691</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.543667</t>
+          <t>2025-10-17T07:09:26.023691</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.543667</t>
+          <t>2025-10-17T07:09:26.025306</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.543667</t>
+          <t>2025-10-17T07:09:26.025306</t>
         </is>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.543667</t>
+          <t>2025-10-17T07:09:26.025824</t>
         </is>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.543667</t>
+          <t>2025-10-17T07:09:26.025841</t>
         </is>
       </c>
     </row>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.543667</t>
+          <t>2025-10-17T07:09:26.025841</t>
         </is>
       </c>
     </row>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.543667</t>
+          <t>2025-10-17T07:09:26.025841</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.544665</t>
+          <t>2025-10-17T07:09:26.025841</t>
         </is>
       </c>
     </row>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.544665</t>
+          <t>2025-10-17T07:09:26.025841</t>
         </is>
       </c>
     </row>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.544665</t>
+          <t>2025-10-17T07:09:26.027192</t>
         </is>
       </c>
     </row>
@@ -1955,7 +1955,7 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.600160</t>
+          <t>2025-10-17T07:09:26.136520</t>
         </is>
       </c>
     </row>
@@ -2045,7 +2045,7 @@
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.601162</t>
+          <t>2025-10-17T07:09:26.136616</t>
         </is>
       </c>
     </row>
@@ -2135,7 +2135,7 @@
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.601162</t>
+          <t>2025-10-17T07:09:26.136616</t>
         </is>
       </c>
     </row>
@@ -2225,7 +2225,7 @@
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.601162</t>
+          <t>2025-10-17T07:09:26.136616</t>
         </is>
       </c>
     </row>
@@ -2315,7 +2315,7 @@
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.601162</t>
+          <t>2025-10-17T07:09:26.136616</t>
         </is>
       </c>
     </row>
@@ -2405,7 +2405,7 @@
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.601162</t>
+          <t>2025-10-17T07:09:26.136616</t>
         </is>
       </c>
     </row>
@@ -2495,7 +2495,7 @@
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.602160</t>
+          <t>2025-10-17T07:09:26.136616</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.602160</t>
+          <t>2025-10-17T07:09:26.136616</t>
         </is>
       </c>
     </row>
@@ -2675,7 +2675,7 @@
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.602160</t>
+          <t>2025-10-17T07:09:26.136616</t>
         </is>
       </c>
     </row>
@@ -2765,7 +2765,7 @@
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.602160</t>
+          <t>2025-10-17T07:09:26.138717</t>
         </is>
       </c>
     </row>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.708207</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -2953,7 +2953,7 @@
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.708207</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.709202</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3141,7 +3141,7 @@
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.709202</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3231,7 +3231,7 @@
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.709202</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.709202</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3415,7 +3415,7 @@
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.709202</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.710203</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.710203</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.710203</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3787,7 +3787,7 @@
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.710203</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.710203</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       <c r="Y38" t="inlineStr"/>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.711201</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -4061,7 +4061,7 @@
       <c r="Y39" t="inlineStr"/>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.711201</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -4155,7 +4155,7 @@
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.711201</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
       <c r="Y41" t="inlineStr"/>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.711201</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.711201</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -4429,7 +4429,7 @@
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.711201</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -4523,7 +4523,7 @@
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.712200</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.712200</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.712200</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -4801,7 +4801,7 @@
       <c r="Y47" t="inlineStr"/>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.712200</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>
@@ -4895,7 +4895,7 @@
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>2025-10-17T02:10:07.712200</t>
+          <t>2025-10-17T07:09:26.244483</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcciones gráficas y de consistencia en PCSMOTE (cache, colores, labels, densidades)
🖼️ Graficador2D:
• Colores de clase fijados para mantener consistencia entre “Original” y “Aumentado”.
• Orden estable de leyendas.
• Soporte directo de nombres_clase pasado como parámetro.

⚙️ GestorCache:
• Corregido ValueError: The truth value of an array with more than one element is ambiguous.
• Ahora se evalúa X_global sin usar operadores booleanos con arrays.

💾 Cache de densidades:
• Evita sobrescribir resultados previos.
• Usa fingerprint de la minoritaria para validar reutilización segura.

🧩 General:
• Mejor manejo de labels en gráficos.
• Logs más limpios y detección estable de densidades previas.
</commit_message>
<xml_diff>
--- a/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_glass_D25_R25_Pentropia.xlsx
+++ b/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_glass_D25_R25_Pentropia.xlsx
@@ -651,7 +651,7 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.023691</t>
+          <t>2025-10-19T23:55:05.901687</t>
         </is>
       </c>
     </row>
@@ -745,7 +745,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.023691</t>
+          <t>2025-10-19T23:55:05.901687</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.023691</t>
+          <t>2025-10-19T23:55:05.901687</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.023691</t>
+          <t>2025-10-19T23:55:05.902688</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.023691</t>
+          <t>2025-10-19T23:55:05.902688</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.025306</t>
+          <t>2025-10-19T23:55:05.902688</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.025306</t>
+          <t>2025-10-19T23:55:05.902688</t>
         </is>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.025824</t>
+          <t>2025-10-19T23:55:05.902688</t>
         </is>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.025841</t>
+          <t>2025-10-19T23:55:05.903687</t>
         </is>
       </c>
     </row>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.025841</t>
+          <t>2025-10-19T23:55:05.903687</t>
         </is>
       </c>
     </row>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.025841</t>
+          <t>2025-10-19T23:55:05.903687</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.025841</t>
+          <t>2025-10-19T23:55:05.903687</t>
         </is>
       </c>
     </row>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.025841</t>
+          <t>2025-10-19T23:55:05.903687</t>
         </is>
       </c>
     </row>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.027192</t>
+          <t>2025-10-19T23:55:05.903687</t>
         </is>
       </c>
     </row>
@@ -1955,7 +1955,7 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.136520</t>
+          <t>2025-10-19T23:55:06.013904</t>
         </is>
       </c>
     </row>
@@ -2045,7 +2045,7 @@
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.136616</t>
+          <t>2025-10-19T23:55:06.013904</t>
         </is>
       </c>
     </row>
@@ -2135,7 +2135,7 @@
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.136616</t>
+          <t>2025-10-19T23:55:06.013904</t>
         </is>
       </c>
     </row>
@@ -2225,7 +2225,7 @@
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.136616</t>
+          <t>2025-10-19T23:55:06.014901</t>
         </is>
       </c>
     </row>
@@ -2315,7 +2315,7 @@
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.136616</t>
+          <t>2025-10-19T23:55:06.014901</t>
         </is>
       </c>
     </row>
@@ -2405,7 +2405,7 @@
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.136616</t>
+          <t>2025-10-19T23:55:06.014901</t>
         </is>
       </c>
     </row>
@@ -2495,7 +2495,7 @@
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.136616</t>
+          <t>2025-10-19T23:55:06.014901</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.136616</t>
+          <t>2025-10-19T23:55:06.014901</t>
         </is>
       </c>
     </row>
@@ -2675,7 +2675,7 @@
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.136616</t>
+          <t>2025-10-19T23:55:06.014901</t>
         </is>
       </c>
     </row>
@@ -2765,7 +2765,7 @@
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.138717</t>
+          <t>2025-10-19T23:55:06.015901</t>
         </is>
       </c>
     </row>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.150310</t>
         </is>
       </c>
     </row>
@@ -2953,7 +2953,7 @@
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.151310</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.151310</t>
         </is>
       </c>
     </row>
@@ -3141,7 +3141,7 @@
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.151310</t>
         </is>
       </c>
     </row>
@@ -3231,7 +3231,7 @@
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.151310</t>
         </is>
       </c>
     </row>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.151310</t>
         </is>
       </c>
     </row>
@@ -3415,7 +3415,7 @@
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.151310</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.152310</t>
         </is>
       </c>
     </row>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.152310</t>
         </is>
       </c>
     </row>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.152310</t>
         </is>
       </c>
     </row>
@@ -3787,7 +3787,7 @@
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.152310</t>
         </is>
       </c>
     </row>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.152310</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       <c r="Y38" t="inlineStr"/>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.152310</t>
         </is>
       </c>
     </row>
@@ -4061,7 +4061,7 @@
       <c r="Y39" t="inlineStr"/>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.153312</t>
         </is>
       </c>
     </row>
@@ -4155,7 +4155,7 @@
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.153312</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
       <c r="Y41" t="inlineStr"/>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.153312</t>
         </is>
       </c>
     </row>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.153312</t>
         </is>
       </c>
     </row>
@@ -4429,7 +4429,7 @@
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.153312</t>
         </is>
       </c>
     </row>
@@ -4523,7 +4523,7 @@
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.153312</t>
         </is>
       </c>
     </row>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.153312</t>
         </is>
       </c>
     </row>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.154313</t>
         </is>
       </c>
     </row>
@@ -4801,7 +4801,7 @@
       <c r="Y47" t="inlineStr"/>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.154313</t>
         </is>
       </c>
     </row>
@@ -4895,7 +4895,7 @@
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>2025-10-17T07:09:26.244483</t>
+          <t>2025-10-19T23:55:06.154313</t>
         </is>
       </c>
     </row>

</xml_diff>